<commit_message>
changed exel input data for freight matrix and milkrun opt plus
</commit_message>
<xml_diff>
--- a/pyloghub/sample_data/MilkrunPlusSampleDataAddresses.xlsx
+++ b/pyloghub/sample_data/MilkrunPlusSampleDataAddresses.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Git\log-hub\log_hub\sample_data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\log-hub-python\pyloghub\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D389AFBD-78F0-4C3C-ADA2-B8BF6900ADF3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60669885-DAF4-4303-8C57-79FC15F8978C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="38620" windowHeight="21100" xr2:uid="{0F815C8C-0ED9-4734-BB11-57244BED7296}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{0F815C8C-0ED9-4734-BB11-57244BED7296}"/>
   </bookViews>
   <sheets>
     <sheet name="breaks" sheetId="7" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="581" uniqueCount="148">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="601" uniqueCount="158">
   <si>
     <t>Depot_Zurich</t>
   </si>
@@ -429,9 +429,6 @@
     <t>speedFactor</t>
   </si>
   <si>
-    <t>fixed</t>
-  </si>
-  <si>
     <t>perHour</t>
   </si>
   <si>
@@ -484,19 +481,64 @@
   </si>
   <si>
     <t>breakDuration</t>
+  </si>
+  <si>
+    <t>B2</t>
+  </si>
+  <si>
+    <t>processingTimeAtTheDepo</t>
+  </si>
+  <si>
+    <t>earliestRelativeBreakStart</t>
+  </si>
+  <si>
+    <t>latestRelativeBreakStart</t>
+  </si>
+  <si>
+    <t>max_distance</t>
+  </si>
+  <si>
+    <t>external_costs</t>
+  </si>
+  <si>
+    <t>perKilometer</t>
+  </si>
+  <si>
+    <t>minimumTravelTime</t>
+  </si>
+  <si>
+    <t>maximumDistanceBetweenStops</t>
+  </si>
+  <si>
+    <t>fixedCostsTO</t>
+  </si>
+  <si>
+    <t>costPerStop</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
     </font>
   </fonts>
   <fills count="2">
@@ -546,34 +588,42 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="6">
+  <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="164" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -589,13 +639,15 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E3CC53F6-89D3-4DA4-AC67-A7FC1E5064A2}" name="Table511" displayName="Table511" ref="A1:E2" totalsRowShown="0">
-  <autoFilter ref="A1:E2" xr:uid="{E3CC53F6-89D3-4DA4-AC67-A7FC1E5064A2}"/>
-  <tableColumns count="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{E3CC53F6-89D3-4DA4-AC67-A7FC1E5064A2}" name="Table511" displayName="Table511" ref="A1:G5" totalsRowShown="0">
+  <autoFilter ref="A1:G5" xr:uid="{E3CC53F6-89D3-4DA4-AC67-A7FC1E5064A2}"/>
+  <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E57E791D-2949-4369-AE80-A717F4977501}" name="id"/>
     <tableColumn id="5" xr3:uid="{BD76FB28-B1C3-49FF-8441-BFD5029F86B0}" name="breakId"/>
-    <tableColumn id="2" xr3:uid="{BE04035B-9895-4FA9-8AC7-E7711538F766}" name="earliestBreakStart" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{5AEC86A9-531E-465D-B647-B28088A9E5CA}" name="latestBreakStart" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{BE04035B-9895-4FA9-8AC7-E7711538F766}" name="earliestBreakStart" dataDxfId="3"/>
+    <tableColumn id="3" xr3:uid="{5AEC86A9-531E-465D-B647-B28088A9E5CA}" name="latestBreakStart" dataDxfId="2"/>
+    <tableColumn id="7" xr3:uid="{1FFB90BB-82E4-4800-8D4E-7A156C0EE645}" name="earliestRelativeBreakStart" dataDxfId="1"/>
+    <tableColumn id="6" xr3:uid="{12EBD8F1-15FE-499B-B3EC-F1010ADC8210}" name="latestRelativeBreakStart" dataDxfId="0"/>
     <tableColumn id="4" xr3:uid="{76775C29-D872-4764-8FD6-A860624EC92C}" name="breakDuration"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -603,9 +655,9 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C42CF9AB-2F6C-40C6-B939-97E3F447AAE3}" name="Table17" displayName="Table17" ref="A1:G2" totalsRowShown="0">
-  <autoFilter ref="A1:G2" xr:uid="{C42CF9AB-2F6C-40C6-B939-97E3F447AAE3}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="6" xr:uid="{C42CF9AB-2F6C-40C6-B939-97E3F447AAE3}" name="Table17" displayName="Table17" ref="A1:H2" totalsRowShown="0">
+  <autoFilter ref="A1:H2" xr:uid="{C42CF9AB-2F6C-40C6-B939-97E3F447AAE3}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{AD28C59A-6E41-489A-A9A1-BE51606DA748}" name="id"/>
     <tableColumn id="7" xr3:uid="{25A09548-6CEF-4909-9FA7-87E6373D802E}" name="depotId"/>
     <tableColumn id="2" xr3:uid="{7AC6530F-CE68-4AC0-9B6B-833537796378}" name="country"/>
@@ -613,15 +665,16 @@
     <tableColumn id="4" xr3:uid="{7A59AE65-32B6-4BAA-8D09-3C1DCC85CA26}" name="postalCode"/>
     <tableColumn id="5" xr3:uid="{8BD6787B-7D04-4FE2-91DC-822C89A1B00E}" name="city"/>
     <tableColumn id="6" xr3:uid="{6BECF5BF-B088-44B4-A52E-95B863260302}" name="street"/>
+    <tableColumn id="8" xr3:uid="{2A3E0DEF-EF5D-429D-9CAD-247B2A1570BB}" name="processingTimeAtTheDepo"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F2A360A2-95C4-441C-9E61-7152940151BA}" name="Table28" displayName="Table28" ref="A1:Q16" totalsRowShown="0">
-  <autoFilter ref="A1:Q16" xr:uid="{F2A360A2-95C4-441C-9E61-7152940151BA}"/>
-  <tableColumns count="17">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{F2A360A2-95C4-441C-9E61-7152940151BA}" name="Table28" displayName="Table28" ref="A1:V16" totalsRowShown="0">
+  <autoFilter ref="A1:V16" xr:uid="{F2A360A2-95C4-441C-9E61-7152940151BA}"/>
+  <tableColumns count="22">
     <tableColumn id="1" xr3:uid="{3DAC24CB-51F8-49E8-9A7A-EB6A8F080BD0}" name="id"/>
     <tableColumn id="17" xr3:uid="{B8DB0140-3581-4086-A644-06E4BB7BEC61}" name="vehicleTypeId"/>
     <tableColumn id="2" xr3:uid="{631BAE15-1192-4896-9ABB-1E7FC0421910}" name="availableVehicles"/>
@@ -631,13 +684,18 @@
     <tableColumn id="6" xr3:uid="{76D73D27-77CF-498A-990C-4BECA6A66082}" name="maxVolume"/>
     <tableColumn id="7" xr3:uid="{97E6D5C9-AA25-44FE-BE71-979D3E8075E3}" name="maxPallets"/>
     <tableColumn id="8" xr3:uid="{D7DDA48A-AD0E-4148-81AD-91A520B28BA0}" name="maxStops"/>
-    <tableColumn id="9" xr3:uid="{8DF1FE6C-BBCD-4B1D-89E5-78D6EBD77E98}" name="timeWindowStart" dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{AA4E50FA-44AD-4DEE-ABFC-F84CDE509891}" name="timeWindowEnd" dataDxfId="2"/>
+    <tableColumn id="9" xr3:uid="{8DF1FE6C-BBCD-4B1D-89E5-78D6EBD77E98}" name="timeWindowStart" dataDxfId="7"/>
+    <tableColumn id="10" xr3:uid="{AA4E50FA-44AD-4DEE-ABFC-F84CDE509891}" name="timeWindowEnd" dataDxfId="6"/>
     <tableColumn id="11" xr3:uid="{F43347B9-3803-4581-9D60-15EA1CBF8049}" name="profile"/>
     <tableColumn id="12" xr3:uid="{1125F421-21B7-48BF-9892-62B15A4C75A5}" name="speedFactor"/>
-    <tableColumn id="13" xr3:uid="{EF8C959B-AD29-49C3-8BC7-C2248CA5EC46}" name="fixed"/>
+    <tableColumn id="13" xr3:uid="{EF8C959B-AD29-49C3-8BC7-C2248CA5EC46}" name="fixedCostsTO"/>
     <tableColumn id="14" xr3:uid="{0320C09B-8370-490B-AE50-E6246943B7C3}" name="perHour"/>
+    <tableColumn id="19" xr3:uid="{62F377B8-BDFE-4C88-A6EF-E480A17D35E1}" name="perKilometer"/>
+    <tableColumn id="18" xr3:uid="{6E69B321-9621-4D6E-B178-6DCCBB90DFCB}" name="costPerStop"/>
+    <tableColumn id="20" xr3:uid="{452E06D8-49E9-4507-A1C2-CF1AAA128698}" name="minimumTravelTime"/>
     <tableColumn id="15" xr3:uid="{F11339F9-CE45-4D42-BD4E-2F2C36D99C51}" name="maxTravelTime"/>
+    <tableColumn id="21" xr3:uid="{DC8ACB6E-8F8C-461D-8DCD-A649709FE30B}" name="max_distance"/>
+    <tableColumn id="22" xr3:uid="{5913B63F-75F2-465F-834B-CC9B6DF2EA37}" name="maximumDistanceBetweenStops"/>
     <tableColumn id="16" xr3:uid="{EE5751D9-C5CE-4B62-8AA3-440B19A8DF05}" name="breakId"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -645,9 +703,9 @@
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADCCD1F6-E2D7-4CEF-A2B0-F425782A4618}" name="Table24" displayName="Table24" ref="A1:P45" totalsRowShown="0">
-  <autoFilter ref="A1:P45" xr:uid="{ADCCD1F6-E2D7-4CEF-A2B0-F425782A4618}"/>
-  <tableColumns count="16">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{ADCCD1F6-E2D7-4CEF-A2B0-F425782A4618}" name="Table24" displayName="Table24" ref="A1:Q45" totalsRowShown="0">
+  <autoFilter ref="A1:Q45" xr:uid="{ADCCD1F6-E2D7-4CEF-A2B0-F425782A4618}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{3EED5214-37BC-4A32-8956-5AC6C29E5C78}" name="id"/>
     <tableColumn id="16" xr3:uid="{FD597778-664E-4AFE-961E-CECAA7BA6B3A}" name="orderId"/>
     <tableColumn id="2" xr3:uid="{10FCEA3F-7DE2-491B-830B-4747A5A2B515}" name="country"/>
@@ -664,6 +722,7 @@
     <tableColumn id="13" xr3:uid="{4D8B07C2-2CD0-47AE-B5F2-DE14A0D1E495}" name="stopDuration"/>
     <tableColumn id="14" xr3:uid="{F659A060-E643-44C3-A792-8818F3219D03}" name="timeWindowProfile"/>
     <tableColumn id="15" xr3:uid="{9A7BEF9E-1B6C-4967-B0BB-E32D14C703CB}" name="stopDurationAtDepot"/>
+    <tableColumn id="17" xr3:uid="{B48DC1DF-0D50-4F85-AAF3-709580CFF340}" name="external_costs"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -675,17 +734,17 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C46AC66F-E99B-4596-BCC5-4402F3E497A7}" name="id"/>
     <tableColumn id="4" xr3:uid="{6B9842D9-BAE2-443C-ABB0-F1EA88103531}" name="timeWindowProfileId"/>
-    <tableColumn id="2" xr3:uid="{53D9870D-FCE3-4A00-A402-D21C5687C4F9}" name="timeWindowProfileStart" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{5BA78898-0159-49D6-AD65-F0036067478E}" name="timeWindowProfileEnd" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{53D9870D-FCE3-4A00-A402-D21C5687C4F9}" name="timeWindowProfileStart" dataDxfId="5"/>
+    <tableColumn id="3" xr3:uid="{5BA78898-0159-49D6-AD65-F0036067478E}" name="timeWindowProfileEnd" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -723,7 +782,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -829,7 +888,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -971,7 +1030,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -979,8 +1038,11 @@
 
 <file path=xl/webextensions/taskpanes.xml><?xml version="1.0" encoding="utf-8"?>
 <wetp:taskpanes xmlns:wetp="http://schemas.microsoft.com/office/webextensions/taskpanes/2010/11">
-  <wetp:taskpane dockstate="right" visibility="0" width="438" row="1">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="5">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+  </wetp:taskpane>
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="7">
+    <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
 </wetp:taskpanes>
 </file>
@@ -992,18 +1054,74 @@
     <we:reference id="WA104381181" version="2.0.0.2" store="" storeType="OMEX"/>
   </we:alternateReferences>
   <we:properties>
-    <we:property name="14_1depots" value="&quot;858b1e05-99efb5cf-9e414fc2&quot;"/>
-    <we:property name="14_1vehicles" value="&quot;cffd3524-cefe18ea-132fb08d&quot;"/>
-    <we:property name="14_1timeWindowProfiles" value="&quot;7d2207a6-f2376535-0c372036&quot;"/>
-    <we:property name="14_1jobs" value="&quot;18282ec6-3e98e863-561fd8ab&quot;"/>
-    <we:property name="14_1breaks" value="&quot;a007269c-ab04e1a8-89169934&quot;"/>
+    <we:property name="14_1breaks" value="&quot;7afbdd87-e4bd867a-3ac1b0a1&quot;"/>
+    <we:property name="14_1depots" value="&quot;3405e038-2cc2c29d-10eabe2d&quot;"/>
+    <we:property name="14_1jobs" value="&quot;e4ebf57b-1d60ebfd-c740eb9d&quot;"/>
+    <we:property name="14_1timeWindowProfiles" value="&quot;f78470fc-c107cc5b-54cc99c0&quot;"/>
+    <we:property name="14_1vehicles" value="&quot;8bf81588-6d943fe2-b4f69674&quot;"/>
+    <we:property name="2_1breaks" value="&quot;6b769a54-c276e826-b41f5dbf&quot;"/>
+    <we:property name="2_1depots" value="&quot;40c7738c-7d0d869f-c5c48545&quot;"/>
+    <we:property name="2_1droppedCustomers" value="&quot;352093c7-c9d2b947-ef8e67d7&quot;"/>
+    <we:property name="2_1jobs" value="&quot;50a46a1f-a10ab40c-f5fab965&quot;"/>
+    <we:property name="2_1parameters" value="&quot;fa6a6550-74c811c1-e51c5e81&quot;"/>
+    <we:property name="2_1routeDetails" value="&quot;39d70381-db5bf02d-2485588d&quot;"/>
+    <we:property name="2_1routeOverview" value="&quot;abd9d53b-efd000b3-a41ffa1f&quot;"/>
+    <we:property name="2_1timeWindowProfiles" value="&quot;05f08bb9-0259b0db-bc32b2ad&quot;"/>
+    <we:property name="2_1vehicles" value="&quot;910a446e-de7f48e3-4d67c1ef&quot;"/>
+    <we:property name="2_3breaks" value="&quot;4db2b91d-d67b452b-d5c01d25&quot;"/>
+    <we:property name="2_3jobs" value="&quot;1a874645-7b386e0a-81502215&quot;"/>
+    <we:property name="2_3timeWindowProfiles" value="&quot;18d160ab-d6668c86-81f62770&quot;"/>
+    <we:property name="2_3vehicles" value="&quot;21ef14b5-164df8cc-9e688600&quot;"/>
   </we:properties>
   <we:bindings>
-    <we:binding id="858b1e05-99efb5cf-9e414fc2" type="table" appref="{DA521017-E136-49AB-95DF-D1981BEFE3B5}"/>
-    <we:binding id="cffd3524-cefe18ea-132fb08d" type="table" appref="{E0A2F988-0AF5-4344-BA1C-AE806D881091}"/>
-    <we:binding id="7d2207a6-f2376535-0c372036" type="table" appref="{A69C37FA-7966-4202-88F6-171633890DA0}"/>
-    <we:binding id="18282ec6-3e98e863-561fd8ab" type="table" appref="{28B51DDE-6AC7-4E1E-9528-60EBBAB976D3}"/>
-    <we:binding id="a007269c-ab04e1a8-89169934" type="table" appref="{6717F94F-D005-400B-8B5E-66834ED751E8}"/>
+    <we:binding id="3405e038-2cc2c29d-10eabe2d" type="table" appref="{EEC9A2D5-5C2E-4DCE-B266-7F94D3DD210B}"/>
+    <we:binding id="8bf81588-6d943fe2-b4f69674" type="table" appref="{C8222C93-A325-412C-B7D9-0552E7CCD631}"/>
+    <we:binding id="e4ebf57b-1d60ebfd-c740eb9d" type="table" appref="{B49F1FF7-7D18-4492-8B49-454159EC6F75}"/>
+    <we:binding id="f78470fc-c107cc5b-54cc99c0" type="table" appref="{20CA339F-A43F-4CB3-B4AE-28B4E8977143}"/>
+    <we:binding id="7afbdd87-e4bd867a-3ac1b0a1" type="table" appref="{88D4A976-03AF-4F97-945E-21395CB42CE5}"/>
+    <we:binding id="21ef14b5-164df8cc-9e688600" type="table" appref="{E60AC61A-415D-4DD1-B29C-8D8A30B74484}"/>
+    <we:binding id="1a874645-7b386e0a-81502215" type="table" appref="{F625127A-070D-457C-AED3-12FF1BFBF57C}"/>
+    <we:binding id="18d160ab-d6668c86-81f62770" type="table" appref="{F1323060-DFBC-49EA-A93E-8C7031B20F51}"/>
+    <we:binding id="4db2b91d-d67b452b-d5c01d25" type="table" appref="{486C6350-B77A-4C63-96A5-7454A2135AC4}"/>
+    <we:binding id="40c7738c-7d0d869f-c5c48545" type="table" appref="{E2CFFF72-7EEF-4987-B318-E23AF7DD55C2}"/>
+    <we:binding id="910a446e-de7f48e3-4d67c1ef" type="table" appref="{CE979D72-3D48-4B73-A4C9-C69944530757}"/>
+    <we:binding id="50a46a1f-a10ab40c-f5fab965" type="table" appref="{89B71074-7E43-4CA4-8F1E-BD90C3E68383}"/>
+    <we:binding id="05f08bb9-0259b0db-bc32b2ad" type="table" appref="{12CD85D8-5F5F-4957-A8E3-475113E9DD6E}"/>
+    <we:binding id="6b769a54-c276e826-b41f5dbf" type="table" appref="{74386F98-86FA-4DBF-AAC5-E42BEE200E06}"/>
+    <we:binding id="abd9d53b-efd000b3-a41ffa1f" type="table" appref="{8628E7A6-0BD3-440F-8A2A-11C4FE56BC46}"/>
+    <we:binding id="39d70381-db5bf02d-2485588d" type="table" appref="{3EB9D26B-B6C7-49DA-9CCE-3BA567A59802}"/>
+    <we:binding id="352093c7-c9d2b947-ef8e67d7" type="table" appref="{BFEB79C1-DF4E-4037-A754-625E127A9F7C}"/>
+    <we:binding id="fa6a6550-74c811c1-e51c5e81" type="table" appref="{A0348EC9-5B47-4B03-834D-97D560693932}"/>
+  </we:bindings>
+  <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
+</we:webextension>
+</file>
+
+<file path=xl/webextensions/webextension2.xml><?xml version="1.0" encoding="utf-8"?>
+<we:webextension xmlns:we="http://schemas.microsoft.com/office/webextensions/webextension/2010/11" id="{8C184108-F20F-42B8-A881-28E7A0FBCF45}">
+  <we:reference id="e504fb41-a92a-4526-b101-542f357b7983" version="1.0.0.0" store="\\LAPTOP-ULOOTDBM\Manifest" storeType="Filesystem"/>
+  <we:alternateReferences/>
+  <we:properties>
+    <we:property name="2_1breaks" value="&quot;bade92af-f7d4abb8-dfbd0975&quot;"/>
+    <we:property name="2_1depots" value="&quot;2c2d3475-cc0c5c3d-f3adb6ec&quot;"/>
+    <we:property name="2_1droppedCustomers" value="&quot;fc401730-040504bf-d448b086&quot;"/>
+    <we:property name="2_1jobs" value="&quot;22f3687a-a1c2606c-83b46295&quot;"/>
+    <we:property name="2_1parameters" value="&quot;44c77af5-a430caf3-1dbe6577&quot;"/>
+    <we:property name="2_1routeDetails" value="&quot;37a755cb-87a0ed7f-a220640d&quot;"/>
+    <we:property name="2_1routeOverview" value="&quot;53b148c5-6be943f6-0b4ca14a&quot;"/>
+    <we:property name="2_1timeWindowProfiles" value="&quot;c2c73dad-e948b378-52853065&quot;"/>
+    <we:property name="2_1vehicles" value="&quot;0ec1d9a8-ce8e9fc6-49dfdcdd&quot;"/>
+  </we:properties>
+  <we:bindings>
+    <we:binding id="2c2d3475-cc0c5c3d-f3adb6ec" type="matrix" appref="{63A1049B-A37B-42B2-83D0-D48F45C21354}"/>
+    <we:binding id="0ec1d9a8-ce8e9fc6-49dfdcdd" type="matrix" appref="{C55476B0-0DB4-446B-AF8D-421E2CD128D7}"/>
+    <we:binding id="22f3687a-a1c2606c-83b46295" type="matrix" appref="{B09183C9-7DA5-430B-9EC5-F08C28B2D708}"/>
+    <we:binding id="c2c73dad-e948b378-52853065" type="matrix" appref="{6322DE5F-8152-4E29-90D0-8A92B177DC60}"/>
+    <we:binding id="bade92af-f7d4abb8-dfbd0975" type="matrix" appref="{5710F216-2749-4C81-A85C-137BDBFBBD2C}"/>
+    <we:binding id="53b148c5-6be943f6-0b4ca14a" type="table" appref="{43A7F7FF-B89E-4C54-97C2-58D1AD93BC65}"/>
+    <we:binding id="fc401730-040504bf-d448b086" type="table" appref="{70DE82A1-4A35-4D9F-828A-CB10E820B8C2}"/>
+    <we:binding id="37a755cb-87a0ed7f-a220640d" type="table" appref="{F11DBFB7-7701-48D3-91F4-293D6D8705B0}"/>
+    <we:binding id="44c77af5-a430caf3-1dbe6577" type="table" appref="{983A8470-2E0A-4B62-B7B1-44C5997C0F9E}"/>
   </we:bindings>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </we:webextension>
@@ -1011,32 +1129,45 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DF8B55EE-9EED-4C08-989B-2652246D5E67}">
-  <dimension ref="A1:E2"/>
+  <dimension ref="A1:G5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E2" sqref="E2"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="3" max="3" width="18" customWidth="1"/>
+    <col min="4" max="4" width="30.77734375" customWidth="1"/>
+    <col min="5" max="5" width="24.44140625" customWidth="1"/>
+    <col min="6" max="6" width="28.33203125" customWidth="1"/>
+    <col min="7" max="7" width="12.109375" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>144</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>145</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>146</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>147</v>
-      </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1044,16 +1175,92 @@
         <v>7</v>
       </c>
       <c r="C2" s="3">
+        <v>44546.833333333299</v>
+      </c>
+      <c r="D2" s="3">
+        <v>44546.875</v>
+      </c>
+      <c r="E2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F2" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G2">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C3" s="3">
         <v>44546.916666666701</v>
       </c>
-      <c r="D2" s="3">
+      <c r="D3" s="3">
         <v>44546.958333333299</v>
       </c>
-      <c r="E2">
+      <c r="E3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>2</v>
+      </c>
+      <c r="G3">
         <v>30</v>
       </c>
     </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>147</v>
+      </c>
+      <c r="C4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D4" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E4" s="5">
+        <v>8.3333333300000006E-2</v>
+      </c>
+      <c r="F4" s="5">
+        <v>0.16666666669999999</v>
+      </c>
+      <c r="G4">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>147</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="E5" s="5">
+        <v>0.25</v>
+      </c>
+      <c r="F5" s="5">
+        <v>0.33333333333333298</v>
+      </c>
+      <c r="G5">
+        <v>30</v>
+      </c>
+    </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -1061,19 +1268,85 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{F7C9EE02-42E1-4005-9D12-6889AFFD525C}">
       <x15:webExtensions xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x15:webExtension appRef="{DA521017-E136-49AB-95DF-D1981BEFE3B5}">
+        <x15:webExtension appRef="{EEC9A2D5-5C2E-4DCE-B266-7F94D3DD210B}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
-        <x15:webExtension appRef="{E0A2F988-0AF5-4344-BA1C-AE806D881091}">
+        <x15:webExtension appRef="{C8222C93-A325-412C-B7D9-0552E7CCD631}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
-        <x15:webExtension appRef="{A69C37FA-7966-4202-88F6-171633890DA0}">
+        <x15:webExtension appRef="{B49F1FF7-7D18-4492-8B49-454159EC6F75}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
-        <x15:webExtension appRef="{28B51DDE-6AC7-4E1E-9528-60EBBAB976D3}">
+        <x15:webExtension appRef="{20CA339F-A43F-4CB3-B4AE-28B4E8977143}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
-        <x15:webExtension appRef="{6717F94F-D005-400B-8B5E-66834ED751E8}">
+        <x15:webExtension appRef="{88D4A976-03AF-4F97-945E-21395CB42CE5}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{E60AC61A-415D-4DD1-B29C-8D8A30B74484}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{F625127A-070D-457C-AED3-12FF1BFBF57C}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{F1323060-DFBC-49EA-A93E-8C7031B20F51}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{486C6350-B77A-4C63-96A5-7454A2135AC4}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{63A1049B-A37B-42B2-83D0-D48F45C21354}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{C55476B0-0DB4-446B-AF8D-421E2CD128D7}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{B09183C9-7DA5-430B-9EC5-F08C28B2D708}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{6322DE5F-8152-4E29-90D0-8A92B177DC60}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{5710F216-2749-4C81-A85C-137BDBFBBD2C}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{43A7F7FF-B89E-4C54-97C2-58D1AD93BC65}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{70DE82A1-4A35-4D9F-828A-CB10E820B8C2}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{F11DBFB7-7701-48D3-91F4-293D6D8705B0}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{983A8470-2E0A-4B62-B7B1-44C5997C0F9E}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{E2CFFF72-7EEF-4987-B318-E23AF7DD55C2}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{CE979D72-3D48-4B73-A4C9-C69944530757}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{89B71074-7E43-4CA4-8F1E-BD90C3E68383}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{12CD85D8-5F5F-4957-A8E3-475113E9DD6E}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{74386F98-86FA-4DBF-AAC5-E42BEE200E06}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{8628E7A6-0BD3-440F-8A2A-11C4FE56BC46}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{3EB9D26B-B6C7-49DA-9CCE-3BA567A59802}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{BFEB79C1-DF4E-4037-A754-625E127A9F7C}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{A0348EC9-5B47-4B03-834D-97D560693932}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
       </x15:webExtensions>
@@ -1084,20 +1357,23 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BD12A80A-2DB3-4011-BFB7-C6CEE8573FA3}">
-  <dimension ref="A1:G2"/>
+  <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="H10" sqref="H10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="8" max="8" width="18.21875" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>112</v>
@@ -1114,8 +1390,11 @@
       <c r="G1" s="2" t="s">
         <v>116</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="H1" s="2" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1136,6 +1415,9 @@
       </c>
       <c r="G2" t="s">
         <v>4</v>
+      </c>
+      <c r="H2">
+        <v>10</v>
       </c>
     </row>
   </sheetData>
@@ -1148,34 +1430,35 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731114BF-9A8C-4E2B-8661-4204E3E4B0F3}">
-  <dimension ref="A1:Q16"/>
+  <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView topLeftCell="C1" workbookViewId="0">
-      <selection activeCell="P2" sqref="P2:P16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E21" sqref="E21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7265625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.88671875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.77734375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="12" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="18.08984375" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="18.6328125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.7265625" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="11.90625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="19.36328125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.36328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="8.6328125" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="13.90625" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.54296875" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10.54296875" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="16.90625" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.109375" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.77734375" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.88671875" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="19.33203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="16.88671875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="10.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:22" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
@@ -1216,19 +1499,34 @@
         <v>128</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="2" t="s">
+        <v>153</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>157</v>
+      </c>
+      <c r="R1" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="S1" s="2" t="s">
         <v>130</v>
       </c>
-      <c r="P1" s="2" t="s">
+      <c r="T1" s="2" t="s">
+        <v>151</v>
+      </c>
+      <c r="U1" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="V1" s="2" t="s">
         <v>131</v>
       </c>
-      <c r="Q1" s="2" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -1275,13 +1573,28 @@
         <v>30</v>
       </c>
       <c r="P2">
-        <v>1200</v>
-      </c>
-      <c r="Q2" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q2">
+        <v>2</v>
+      </c>
+      <c r="R2">
+        <v>2</v>
+      </c>
+      <c r="S2">
+        <v>1000</v>
+      </c>
+      <c r="T2">
+        <v>150</v>
+      </c>
+      <c r="U2">
+        <v>100</v>
+      </c>
+      <c r="V2" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -1328,13 +1641,28 @@
         <v>30</v>
       </c>
       <c r="P3">
-        <v>1200</v>
-      </c>
-      <c r="Q3" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q3">
+        <v>2</v>
+      </c>
+      <c r="R3">
+        <v>2</v>
+      </c>
+      <c r="S3">
+        <v>1000</v>
+      </c>
+      <c r="T3">
+        <v>150</v>
+      </c>
+      <c r="U3">
+        <v>100</v>
+      </c>
+      <c r="V3" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -1381,13 +1709,28 @@
         <v>30</v>
       </c>
       <c r="P4">
-        <v>1200</v>
-      </c>
-      <c r="Q4" t="s">
+        <v>1</v>
+      </c>
+      <c r="Q4">
+        <v>2</v>
+      </c>
+      <c r="R4">
+        <v>2</v>
+      </c>
+      <c r="S4">
+        <v>1000</v>
+      </c>
+      <c r="T4">
+        <v>150</v>
+      </c>
+      <c r="U4">
+        <v>100</v>
+      </c>
+      <c r="V4" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -1434,13 +1777,28 @@
         <v>30</v>
       </c>
       <c r="P5">
-        <v>1200</v>
-      </c>
-      <c r="Q5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q5">
+        <v>2</v>
+      </c>
+      <c r="R5">
+        <v>2</v>
+      </c>
+      <c r="S5">
+        <v>1000</v>
+      </c>
+      <c r="T5">
+        <v>150</v>
+      </c>
+      <c r="U5">
+        <v>100</v>
+      </c>
+      <c r="V5" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -1487,13 +1845,28 @@
         <v>30</v>
       </c>
       <c r="P6">
-        <v>1200</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q6">
+        <v>2</v>
+      </c>
+      <c r="R6">
+        <v>2</v>
+      </c>
+      <c r="S6">
+        <v>1000</v>
+      </c>
+      <c r="T6">
+        <v>150</v>
+      </c>
+      <c r="U6">
+        <v>100</v>
+      </c>
+      <c r="V6" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="7" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -1540,13 +1913,28 @@
         <v>30</v>
       </c>
       <c r="P7">
-        <v>1200</v>
-      </c>
-      <c r="Q7" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q7">
+        <v>2</v>
+      </c>
+      <c r="R7">
+        <v>2</v>
+      </c>
+      <c r="S7">
+        <v>1000</v>
+      </c>
+      <c r="T7">
+        <v>150</v>
+      </c>
+      <c r="U7">
+        <v>100</v>
+      </c>
+      <c r="V7" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="8" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -1593,13 +1981,28 @@
         <v>30</v>
       </c>
       <c r="P8">
-        <v>1200</v>
-      </c>
-      <c r="Q8" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q8">
+        <v>2</v>
+      </c>
+      <c r="R8">
+        <v>2</v>
+      </c>
+      <c r="S8">
+        <v>1000</v>
+      </c>
+      <c r="T8">
+        <v>150</v>
+      </c>
+      <c r="U8">
+        <v>100</v>
+      </c>
+      <c r="V8" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="9" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -1646,13 +2049,28 @@
         <v>30</v>
       </c>
       <c r="P9">
-        <v>1200</v>
-      </c>
-      <c r="Q9" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q9">
+        <v>2</v>
+      </c>
+      <c r="R9">
+        <v>2</v>
+      </c>
+      <c r="S9">
+        <v>1000</v>
+      </c>
+      <c r="T9">
+        <v>150</v>
+      </c>
+      <c r="U9">
+        <v>100</v>
+      </c>
+      <c r="V9" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="10" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -1699,13 +2117,28 @@
         <v>30</v>
       </c>
       <c r="P10">
-        <v>1200</v>
-      </c>
-      <c r="Q10" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q10">
+        <v>2</v>
+      </c>
+      <c r="R10">
+        <v>2</v>
+      </c>
+      <c r="S10">
+        <v>1000</v>
+      </c>
+      <c r="T10">
+        <v>150</v>
+      </c>
+      <c r="U10">
+        <v>100</v>
+      </c>
+      <c r="V10" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -1752,13 +2185,28 @@
         <v>30</v>
       </c>
       <c r="P11">
-        <v>1200</v>
-      </c>
-      <c r="Q11" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q11">
+        <v>2</v>
+      </c>
+      <c r="R11">
+        <v>2</v>
+      </c>
+      <c r="S11">
+        <v>1000</v>
+      </c>
+      <c r="T11">
+        <v>150</v>
+      </c>
+      <c r="U11">
+        <v>100</v>
+      </c>
+      <c r="V11" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="12" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -1805,13 +2253,28 @@
         <v>30</v>
       </c>
       <c r="P12">
-        <v>1200</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q12">
+        <v>2</v>
+      </c>
+      <c r="R12">
+        <v>2</v>
+      </c>
+      <c r="S12">
+        <v>1000</v>
+      </c>
+      <c r="T12">
+        <v>150</v>
+      </c>
+      <c r="U12">
+        <v>100</v>
+      </c>
+      <c r="V12" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="13" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -1858,13 +2321,28 @@
         <v>30</v>
       </c>
       <c r="P13">
-        <v>1200</v>
-      </c>
-      <c r="Q13" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q13">
+        <v>2</v>
+      </c>
+      <c r="R13">
+        <v>2</v>
+      </c>
+      <c r="S13">
+        <v>1000</v>
+      </c>
+      <c r="T13">
+        <v>150</v>
+      </c>
+      <c r="U13">
+        <v>100</v>
+      </c>
+      <c r="V13" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -1911,13 +2389,28 @@
         <v>30</v>
       </c>
       <c r="P14">
-        <v>1200</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q14">
+        <v>2</v>
+      </c>
+      <c r="R14">
+        <v>2</v>
+      </c>
+      <c r="S14">
+        <v>1000</v>
+      </c>
+      <c r="T14">
+        <v>150</v>
+      </c>
+      <c r="U14">
+        <v>100</v>
+      </c>
+      <c r="V14" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="15" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -1964,13 +2457,28 @@
         <v>30</v>
       </c>
       <c r="P15">
-        <v>1200</v>
-      </c>
-      <c r="Q15" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.35">
+        <v>1</v>
+      </c>
+      <c r="Q15">
+        <v>2</v>
+      </c>
+      <c r="R15">
+        <v>2</v>
+      </c>
+      <c r="S15">
+        <v>1000</v>
+      </c>
+      <c r="T15">
+        <v>150</v>
+      </c>
+      <c r="U15">
+        <v>100</v>
+      </c>
+      <c r="V15" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:22" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2017,13 +2525,32 @@
         <v>30</v>
       </c>
       <c r="P16">
-        <v>1200</v>
-      </c>
-      <c r="Q16" t="s">
-        <v>2</v>
-      </c>
+        <v>1</v>
+      </c>
+      <c r="Q16">
+        <v>2</v>
+      </c>
+      <c r="R16">
+        <v>2</v>
+      </c>
+      <c r="S16">
+        <v>1000</v>
+      </c>
+      <c r="T16">
+        <v>150</v>
+      </c>
+      <c r="U16">
+        <v>100</v>
+      </c>
+      <c r="V16" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="23" spans="15:15" x14ac:dyDescent="0.3">
+      <c r="O23" s="6"/>
     </row>
   </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -2033,24 +2560,31 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E9840B-7203-4504-8A3D-5B22E03396E5}">
-  <dimension ref="A1:P45"/>
+  <dimension ref="A1:Q45"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="P2" sqref="P2"/>
+      <selection activeCell="B2" sqref="B2:Q45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="2" max="2" width="14.08984375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="18.44140625" customWidth="1"/>
+    <col min="7" max="7" width="15.44140625" customWidth="1"/>
+    <col min="11" max="11" width="15.5546875" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="15.33203125" customWidth="1"/>
+    <col min="13" max="13" width="14.21875" customWidth="1"/>
+    <col min="14" max="14" width="14" customWidth="1"/>
+    <col min="15" max="15" width="18" customWidth="1"/>
+    <col min="16" max="16" width="13.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:17" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>111</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>112</v>
@@ -2068,34 +2602,37 @@
         <v>116</v>
       </c>
       <c r="H1" s="2" t="s">
+        <v>133</v>
+      </c>
+      <c r="I1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="J1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="J1" s="2" t="s">
+      <c r="K1" s="1" t="s">
         <v>136</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>137</v>
-      </c>
-      <c r="L1" s="1" t="s">
-        <v>138</v>
       </c>
       <c r="M1" s="2" t="s">
         <v>117</v>
       </c>
       <c r="N1" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="O1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="O1" s="2" t="s">
+      <c r="P1" s="6" t="s">
         <v>140</v>
       </c>
-      <c r="P1" s="2" t="s">
-        <v>141</v>
-      </c>
-    </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="Q1" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -2118,10 +2655,10 @@
         <v>18</v>
       </c>
       <c r="H2">
-        <v>336</v>
+        <v>1743</v>
       </c>
       <c r="I2">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J2">
         <v>7</v>
@@ -2142,10 +2679,13 @@
         <v>11</v>
       </c>
       <c r="P2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+        <v>3.5</v>
+      </c>
+      <c r="Q2">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -2168,10 +2708,10 @@
         <v>21</v>
       </c>
       <c r="H3">
-        <v>204</v>
+        <v>1542</v>
       </c>
       <c r="I3">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J3">
         <v>6</v>
@@ -2192,10 +2732,13 @@
         <v>11</v>
       </c>
       <c r="P3">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="Q3">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -2218,10 +2761,10 @@
         <v>23</v>
       </c>
       <c r="H4">
-        <v>460</v>
+        <v>2600</v>
       </c>
       <c r="I4">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J4">
         <v>10</v>
@@ -2242,10 +2785,13 @@
         <v>11</v>
       </c>
       <c r="P4">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="Q4">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -2268,10 +2814,10 @@
         <v>25</v>
       </c>
       <c r="H5">
-        <v>360</v>
+        <v>2032</v>
       </c>
       <c r="I5">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J5">
         <v>8</v>
@@ -2292,10 +2838,13 @@
         <v>11</v>
       </c>
       <c r="P5">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="Q5">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -2318,10 +2867,10 @@
         <v>27</v>
       </c>
       <c r="H6">
-        <v>301</v>
+        <v>1708</v>
       </c>
       <c r="I6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J6">
         <v>7</v>
@@ -2342,10 +2891,13 @@
         <v>11</v>
       </c>
       <c r="P6">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+        <v>3.5</v>
+      </c>
+      <c r="Q6">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -2368,10 +2920,10 @@
         <v>29</v>
       </c>
       <c r="H7">
-        <v>564</v>
+        <v>2856</v>
       </c>
       <c r="I7">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J7">
         <v>12</v>
@@ -2392,10 +2944,13 @@
         <v>11</v>
       </c>
       <c r="P7">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="Q7">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -2418,10 +2973,10 @@
         <v>31</v>
       </c>
       <c r="H8">
-        <v>240</v>
+        <v>1325</v>
       </c>
       <c r="I8">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J8">
         <v>5</v>
@@ -2442,10 +2997,13 @@
         <v>11</v>
       </c>
       <c r="P8">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+        <v>2.5</v>
+      </c>
+      <c r="Q8">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -2468,10 +3026,10 @@
         <v>33</v>
       </c>
       <c r="H9">
-        <v>245</v>
+        <v>1764</v>
       </c>
       <c r="I9">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J9">
         <v>7</v>
@@ -2492,10 +3050,13 @@
         <v>11</v>
       </c>
       <c r="P9">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+        <v>3.5</v>
+      </c>
+      <c r="Q9">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -2518,10 +3079,10 @@
         <v>35</v>
       </c>
       <c r="H10">
-        <v>492</v>
+        <v>3036</v>
       </c>
       <c r="I10">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J10">
         <v>12</v>
@@ -2542,10 +3103,13 @@
         <v>11</v>
       </c>
       <c r="P10">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="Q10">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -2568,10 +3132,10 @@
         <v>37</v>
       </c>
       <c r="H11">
-        <v>450</v>
+        <v>2304</v>
       </c>
       <c r="I11">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J11">
         <v>9</v>
@@ -2592,10 +3156,13 @@
         <v>11</v>
       </c>
       <c r="P11">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.5</v>
+      </c>
+      <c r="Q11">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>11</v>
       </c>
@@ -2618,10 +3185,10 @@
         <v>40</v>
       </c>
       <c r="H12">
-        <v>324</v>
+        <v>2115</v>
       </c>
       <c r="I12">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J12">
         <v>9</v>
@@ -2642,10 +3209,13 @@
         <v>12</v>
       </c>
       <c r="P12">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.5</v>
+      </c>
+      <c r="Q12">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>12</v>
       </c>
@@ -2668,10 +3238,10 @@
         <v>42</v>
       </c>
       <c r="H13">
-        <v>540</v>
+        <v>2784</v>
       </c>
       <c r="I13">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J13">
         <v>12</v>
@@ -2692,10 +3262,13 @@
         <v>12</v>
       </c>
       <c r="P13">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="Q13">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>13</v>
       </c>
@@ -2718,10 +3291,10 @@
         <v>42</v>
       </c>
       <c r="H14">
-        <v>324</v>
+        <v>2106</v>
       </c>
       <c r="I14">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J14">
         <v>9</v>
@@ -2742,10 +3315,13 @@
         <v>12</v>
       </c>
       <c r="P14">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.5</v>
+      </c>
+      <c r="Q14">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>14</v>
       </c>
@@ -2768,10 +3344,10 @@
         <v>45</v>
       </c>
       <c r="H15">
-        <v>360</v>
+        <v>2892</v>
       </c>
       <c r="I15">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J15">
         <v>12</v>
@@ -2792,10 +3368,13 @@
         <v>12</v>
       </c>
       <c r="P15">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="Q15">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>15</v>
       </c>
@@ -2818,10 +3397,10 @@
         <v>47</v>
       </c>
       <c r="H16">
-        <v>344</v>
+        <v>1912</v>
       </c>
       <c r="I16">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J16">
         <v>8</v>
@@ -2842,10 +3421,13 @@
         <v>12</v>
       </c>
       <c r="P16">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="Q16">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>16</v>
       </c>
@@ -2868,10 +3450,10 @@
         <v>49</v>
       </c>
       <c r="H17">
-        <v>160</v>
+        <v>1028</v>
       </c>
       <c r="I17">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J17">
         <v>4</v>
@@ -2892,10 +3474,13 @@
         <v>12</v>
       </c>
       <c r="P17">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="Q17">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>17</v>
       </c>
@@ -2918,10 +3503,10 @@
         <v>51</v>
       </c>
       <c r="H18">
-        <v>363</v>
+        <v>2706</v>
       </c>
       <c r="I18">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J18">
         <v>11</v>
@@ -2942,10 +3527,13 @@
         <v>12</v>
       </c>
       <c r="P18">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+        <v>5.5</v>
+      </c>
+      <c r="Q18">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>18</v>
       </c>
@@ -2968,10 +3556,10 @@
         <v>53</v>
       </c>
       <c r="H19">
-        <v>324</v>
+        <v>2376</v>
       </c>
       <c r="I19">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J19">
         <v>9</v>
@@ -2992,10 +3580,13 @@
         <v>12</v>
       </c>
       <c r="P19">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.5</v>
+      </c>
+      <c r="Q19">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>19</v>
       </c>
@@ -3018,10 +3609,10 @@
         <v>55</v>
       </c>
       <c r="H20">
-        <v>90</v>
+        <v>771</v>
       </c>
       <c r="I20">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J20">
         <v>3</v>
@@ -3042,10 +3633,13 @@
         <v>12</v>
       </c>
       <c r="P20">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.5</v>
+      </c>
+      <c r="Q20">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>20</v>
       </c>
@@ -3068,10 +3662,10 @@
         <v>57</v>
       </c>
       <c r="H21">
-        <v>430</v>
+        <v>2480</v>
       </c>
       <c r="I21">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J21">
         <v>10</v>
@@ -3092,10 +3686,13 @@
         <v>12</v>
       </c>
       <c r="P21">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="Q21">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>21</v>
       </c>
@@ -3118,10 +3715,10 @@
         <v>60</v>
       </c>
       <c r="H22">
-        <v>550</v>
+        <v>2849</v>
       </c>
       <c r="I22">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J22">
         <v>11</v>
@@ -3142,10 +3739,13 @@
         <v>13</v>
       </c>
       <c r="P22">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+        <v>5.5</v>
+      </c>
+      <c r="Q22">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>22</v>
       </c>
@@ -3168,10 +3768,10 @@
         <v>18</v>
       </c>
       <c r="H23">
-        <v>231</v>
+        <v>1757</v>
       </c>
       <c r="I23">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J23">
         <v>7</v>
@@ -3192,10 +3792,13 @@
         <v>13</v>
       </c>
       <c r="P23">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+        <v>3.5</v>
+      </c>
+      <c r="Q23">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>23</v>
       </c>
@@ -3218,10 +3821,10 @@
         <v>64</v>
       </c>
       <c r="H24">
-        <v>336</v>
+        <v>1764</v>
       </c>
       <c r="I24">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J24">
         <v>7</v>
@@ -3242,10 +3845,13 @@
         <v>13</v>
       </c>
       <c r="P24">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+        <v>3.5</v>
+      </c>
+      <c r="Q24">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A25">
         <v>24</v>
       </c>
@@ -3268,10 +3874,10 @@
         <v>66</v>
       </c>
       <c r="H25">
-        <v>170</v>
+        <v>1290</v>
       </c>
       <c r="I25">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J25">
         <v>5</v>
@@ -3292,10 +3898,13 @@
         <v>13</v>
       </c>
       <c r="P25">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+        <v>2.5</v>
+      </c>
+      <c r="Q25">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A26">
         <v>25</v>
       </c>
@@ -3318,10 +3927,10 @@
         <v>69</v>
       </c>
       <c r="H26">
-        <v>190</v>
+        <v>1320</v>
       </c>
       <c r="I26">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J26">
         <v>5</v>
@@ -3342,10 +3951,13 @@
         <v>13</v>
       </c>
       <c r="P26">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+        <v>2.5</v>
+      </c>
+      <c r="Q26">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A27">
         <v>26</v>
       </c>
@@ -3368,10 +3980,10 @@
         <v>40</v>
       </c>
       <c r="H27">
-        <v>500</v>
+        <v>2300</v>
       </c>
       <c r="I27">
-        <v>1</v>
+        <v>8</v>
       </c>
       <c r="J27">
         <v>10</v>
@@ -3392,10 +4004,13 @@
         <v>13</v>
       </c>
       <c r="P27">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+        <v>5</v>
+      </c>
+      <c r="Q27">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A28">
         <v>27</v>
       </c>
@@ -3418,10 +4033,10 @@
         <v>73</v>
       </c>
       <c r="H28">
-        <v>378</v>
+        <v>2214</v>
       </c>
       <c r="I28">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J28">
         <v>9</v>
@@ -3442,10 +4057,13 @@
         <v>13</v>
       </c>
       <c r="P28">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.5</v>
+      </c>
+      <c r="Q28">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A29">
         <v>28</v>
       </c>
@@ -3468,10 +4086,10 @@
         <v>18</v>
       </c>
       <c r="H29">
-        <v>185</v>
+        <v>1340</v>
       </c>
       <c r="I29">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J29">
         <v>5</v>
@@ -3492,10 +4110,13 @@
         <v>13</v>
       </c>
       <c r="P29">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+        <v>2.5</v>
+      </c>
+      <c r="Q29">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A30">
         <v>29</v>
       </c>
@@ -3518,10 +4139,10 @@
         <v>77</v>
       </c>
       <c r="H30">
-        <v>156</v>
+        <v>1036</v>
       </c>
       <c r="I30">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="J30">
         <v>4</v>
@@ -3542,10 +4163,13 @@
         <v>14</v>
       </c>
       <c r="P30">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+        <v>2</v>
+      </c>
+      <c r="Q30">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A31">
         <v>30</v>
       </c>
@@ -3568,10 +4192,10 @@
         <v>79</v>
       </c>
       <c r="H31">
-        <v>306</v>
+        <v>2349</v>
       </c>
       <c r="I31">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J31">
         <v>9</v>
@@ -3592,10 +4216,13 @@
         <v>14</v>
       </c>
       <c r="P31">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.5</v>
+      </c>
+      <c r="Q31">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A32">
         <v>31</v>
       </c>
@@ -3618,10 +4245,10 @@
         <v>81</v>
       </c>
       <c r="H32">
-        <v>150</v>
+        <v>729</v>
       </c>
       <c r="I32">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J32">
         <v>3</v>
@@ -3642,10 +4269,13 @@
         <v>14</v>
       </c>
       <c r="P32">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.5</v>
+      </c>
+      <c r="Q32">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="33" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A33">
         <v>32</v>
       </c>
@@ -3668,10 +4298,10 @@
         <v>84</v>
       </c>
       <c r="H33">
-        <v>441</v>
+        <v>2403</v>
       </c>
       <c r="I33">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J33">
         <v>9</v>
@@ -3692,10 +4322,13 @@
         <v>14</v>
       </c>
       <c r="P33">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.5</v>
+      </c>
+      <c r="Q33">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="34" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A34">
         <v>33</v>
       </c>
@@ -3718,10 +4351,10 @@
         <v>87</v>
       </c>
       <c r="H34">
-        <v>117</v>
+        <v>759</v>
       </c>
       <c r="I34">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J34">
         <v>3</v>
@@ -3742,10 +4375,13 @@
         <v>14</v>
       </c>
       <c r="P34">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+        <v>1.5</v>
+      </c>
+      <c r="Q34">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="35" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A35">
         <v>34</v>
       </c>
@@ -3768,10 +4404,10 @@
         <v>89</v>
       </c>
       <c r="H35">
-        <v>272</v>
+        <v>2064</v>
       </c>
       <c r="I35">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J35">
         <v>8</v>
@@ -3792,10 +4428,13 @@
         <v>14</v>
       </c>
       <c r="P35">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4</v>
+      </c>
+      <c r="Q35">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="36" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A36">
         <v>35</v>
       </c>
@@ -3818,10 +4457,10 @@
         <v>91</v>
       </c>
       <c r="H36">
-        <v>273</v>
+        <v>1610</v>
       </c>
       <c r="I36">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="J36">
         <v>7</v>
@@ -3842,10 +4481,13 @@
         <v>14</v>
       </c>
       <c r="P36">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+        <v>3.5</v>
+      </c>
+      <c r="Q36">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="37" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A37">
         <v>36</v>
       </c>
@@ -3868,10 +4510,10 @@
         <v>94</v>
       </c>
       <c r="H37">
-        <v>441</v>
+        <v>2385</v>
       </c>
       <c r="I37">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J37">
         <v>9</v>
@@ -3892,10 +4534,13 @@
         <v>15</v>
       </c>
       <c r="P37">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.5</v>
+      </c>
+      <c r="Q37">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="38" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>37</v>
       </c>
@@ -3918,10 +4563,10 @@
         <v>96</v>
       </c>
       <c r="H38">
-        <v>216</v>
+        <v>1536</v>
       </c>
       <c r="I38">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J38">
         <v>6</v>
@@ -3942,10 +4587,13 @@
         <v>15</v>
       </c>
       <c r="P38">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="Q38">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="39" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>38</v>
       </c>
@@ -3968,10 +4616,10 @@
         <v>98</v>
       </c>
       <c r="H39">
-        <v>300</v>
+        <v>1572</v>
       </c>
       <c r="I39">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="J39">
         <v>6</v>
@@ -3992,10 +4640,13 @@
         <v>15</v>
       </c>
       <c r="P39">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+        <v>3</v>
+      </c>
+      <c r="Q39">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="40" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>39</v>
       </c>
@@ -4018,10 +4669,10 @@
         <v>100</v>
       </c>
       <c r="H40">
-        <v>432</v>
+        <v>2106</v>
       </c>
       <c r="I40">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="J40">
         <v>9</v>
@@ -4042,10 +4693,13 @@
         <v>15</v>
       </c>
       <c r="P40">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+        <v>4.5</v>
+      </c>
+      <c r="Q40">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="41" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>40</v>
       </c>
@@ -4068,10 +4722,10 @@
         <v>102</v>
       </c>
       <c r="H41">
-        <v>468</v>
+        <v>3024</v>
       </c>
       <c r="I41">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="J41">
         <v>12</v>
@@ -4092,10 +4746,13 @@
         <v>15</v>
       </c>
       <c r="P41">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+        <v>6</v>
+      </c>
+      <c r="Q41">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="42" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>41</v>
       </c>
@@ -4118,10 +4775,10 @@
         <v>104</v>
       </c>
       <c r="H42">
-        <v>473</v>
+        <v>2739</v>
       </c>
       <c r="I42">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J42">
         <v>11</v>
@@ -4142,10 +4799,13 @@
         <v>15</v>
       </c>
       <c r="P42">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+        <v>5.5</v>
+      </c>
+      <c r="Q42">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="43" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>42</v>
       </c>
@@ -4168,10 +4828,10 @@
         <v>107</v>
       </c>
       <c r="H43">
-        <v>462</v>
+        <v>2651</v>
       </c>
       <c r="I43">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="J43">
         <v>11</v>
@@ -4192,10 +4852,13 @@
         <v>15</v>
       </c>
       <c r="P43">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+        <v>5.5</v>
+      </c>
+      <c r="Q43">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="44" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A44">
         <v>43</v>
       </c>
@@ -4218,10 +4881,10 @@
         <v>107</v>
       </c>
       <c r="H44">
-        <v>170</v>
+        <v>1185</v>
       </c>
       <c r="I44">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="J44">
         <v>5</v>
@@ -4242,10 +4905,13 @@
         <v>15</v>
       </c>
       <c r="P44">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+        <v>2.5</v>
+      </c>
+      <c r="Q44">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="45" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A45">
         <v>44</v>
       </c>
@@ -4268,10 +4934,10 @@
         <v>40</v>
       </c>
       <c r="H45">
-        <v>111</v>
+        <v>792</v>
       </c>
       <c r="I45">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="J45">
         <v>3</v>
@@ -4292,7 +4958,10 @@
         <v>15</v>
       </c>
       <c r="P45">
-        <v>33</v>
+        <v>1.5</v>
+      </c>
+      <c r="Q45">
+        <v>1000</v>
       </c>
     </row>
   </sheetData>
@@ -4307,33 +4976,33 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DC451B-53B4-41CD-9364-638505779A88}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E23" sqref="E23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:D11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="20.7265625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="20.7265625" customWidth="1"/>
-    <col min="3" max="3" width="25.36328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="24.453125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="20.77734375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="20.77734375" customWidth="1"/>
+    <col min="3" max="3" width="25.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="24.44140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" ht="15" thickTop="1" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>111</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>142</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>143</v>
       </c>
-      <c r="D1" s="2" t="s">
-        <v>144</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>1</v>
       </c>
@@ -4347,7 +5016,7 @@
         <v>44547.020833333299</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>2</v>
       </c>
@@ -4361,7 +5030,7 @@
         <v>44547.208333333299</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3</v>
       </c>
@@ -4375,7 +5044,7 @@
         <v>44548.020833333299</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>4</v>
       </c>
@@ -4389,7 +5058,7 @@
         <v>44548.208333333299</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>5</v>
       </c>
@@ -4403,7 +5072,7 @@
         <v>44549.020833333299</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>6</v>
       </c>
@@ -4417,7 +5086,7 @@
         <v>44549.208333333299</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>7</v>
       </c>
@@ -4431,7 +5100,7 @@
         <v>44550.020833333299</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>8</v>
       </c>
@@ -4445,7 +5114,7 @@
         <v>44550.208333333299</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>9</v>
       </c>
@@ -4459,7 +5128,7 @@
         <v>44551.020833333299</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>10</v>
       </c>
@@ -4482,15 +5151,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
   <documentManagement>
     <_activity xmlns="1bb9a224-31c7-42e8-a065-e7e76b1c03c9" xsi:nil="true"/>
@@ -4498,7 +5158,7 @@
 </p:properties>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Dokument" ma:contentTypeID="0x010100FE98BBDBD67EAA48878DDE6E7ACD86CC" ma:contentTypeVersion="13" ma:contentTypeDescription="Ein neues Dokument erstellen." ma:contentTypeScope="" ma:versionID="7a64d83715acf84af5f721f1ddbf92ee">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="15a9d969-c72e-439c-8c09-437e8295500b" xmlns:ns4="1bb9a224-31c7-42e8-a065-e7e76b1c03c9" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="3e469312e1f69fcf92aa8a74229e95fc" ns3:_="" ns4:_="">
     <xsd:import namespace="15a9d969-c72e-439c-8c09-437e8295500b"/>
@@ -4719,15 +5379,16 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1031B672-90B3-497E-AD74-4A5D391605E1}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B9BDB6-33A2-4400-8419-C415F30CCE55}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="1bb9a224-31c7-42e8-a065-e7e76b1c03c9"/>
@@ -4744,7 +5405,7 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5AD5FCE6-ECEA-4808-9CE2-C11F0DA21504}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4761,4 +5422,12 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1031B672-90B3-497E-AD74-4A5D391605E1}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
added missing columns to the input tables in milkrun plus
</commit_message>
<xml_diff>
--- a/pyloghub/sample_data/MilkrunPlusSampleDataAddresses.xlsx
+++ b/pyloghub/sample_data/MilkrunPlusSampleDataAddresses.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\log-hub-python\pyloghub\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60669885-DAF4-4303-8C57-79FC15F8978C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AAAB2A-C4F1-44BF-88AA-38EEA1D4E70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{0F815C8C-0ED9-4734-BB11-57244BED7296}"/>
   </bookViews>
@@ -462,9 +462,6 @@
     <t>timeWindowProfile</t>
   </si>
   <si>
-    <t>stopDurationAtDepot</t>
-  </si>
-  <si>
     <t>timeWindowProfileId</t>
   </si>
   <si>
@@ -514,13 +511,16 @@
   </si>
   <si>
     <t>costPerStop</t>
+  </si>
+  <si>
+    <t>stopDurationAtDepo</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -536,6 +536,12 @@
     </font>
     <font>
       <sz val="8"/>
+      <color theme="1"/>
+      <name val="Consolas"/>
+      <family val="3"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color theme="1"/>
       <name val="Consolas"/>
       <family val="3"/>
@@ -588,7 +594,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
@@ -596,16 +602,14 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="21" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="8">
     <dxf>
-      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
@@ -617,7 +621,10 @@
       <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="26" formatCode="h:mm:ss"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="27" formatCode="m/d/yyyy\ h:mm"/>
@@ -644,10 +651,10 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{E57E791D-2949-4369-AE80-A717F4977501}" name="id"/>
     <tableColumn id="5" xr3:uid="{BD76FB28-B1C3-49FF-8441-BFD5029F86B0}" name="breakId"/>
-    <tableColumn id="2" xr3:uid="{BE04035B-9895-4FA9-8AC7-E7711538F766}" name="earliestBreakStart" dataDxfId="3"/>
-    <tableColumn id="3" xr3:uid="{5AEC86A9-531E-465D-B647-B28088A9E5CA}" name="latestBreakStart" dataDxfId="2"/>
-    <tableColumn id="7" xr3:uid="{1FFB90BB-82E4-4800-8D4E-7A156C0EE645}" name="earliestRelativeBreakStart" dataDxfId="1"/>
-    <tableColumn id="6" xr3:uid="{12EBD8F1-15FE-499B-B3EC-F1010ADC8210}" name="latestRelativeBreakStart" dataDxfId="0"/>
+    <tableColumn id="2" xr3:uid="{BE04035B-9895-4FA9-8AC7-E7711538F766}" name="earliestBreakStart" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{5AEC86A9-531E-465D-B647-B28088A9E5CA}" name="latestBreakStart" dataDxfId="6"/>
+    <tableColumn id="7" xr3:uid="{1FFB90BB-82E4-4800-8D4E-7A156C0EE645}" name="earliestRelativeBreakStart" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{12EBD8F1-15FE-499B-B3EC-F1010ADC8210}" name="latestRelativeBreakStart" dataDxfId="4"/>
     <tableColumn id="4" xr3:uid="{76775C29-D872-4764-8FD6-A860624EC92C}" name="breakDuration"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -684,8 +691,8 @@
     <tableColumn id="6" xr3:uid="{76D73D27-77CF-498A-990C-4BECA6A66082}" name="maxVolume"/>
     <tableColumn id="7" xr3:uid="{97E6D5C9-AA25-44FE-BE71-979D3E8075E3}" name="maxPallets"/>
     <tableColumn id="8" xr3:uid="{D7DDA48A-AD0E-4148-81AD-91A520B28BA0}" name="maxStops"/>
-    <tableColumn id="9" xr3:uid="{8DF1FE6C-BBCD-4B1D-89E5-78D6EBD77E98}" name="timeWindowStart" dataDxfId="7"/>
-    <tableColumn id="10" xr3:uid="{AA4E50FA-44AD-4DEE-ABFC-F84CDE509891}" name="timeWindowEnd" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{8DF1FE6C-BBCD-4B1D-89E5-78D6EBD77E98}" name="timeWindowStart" dataDxfId="3"/>
+    <tableColumn id="10" xr3:uid="{AA4E50FA-44AD-4DEE-ABFC-F84CDE509891}" name="timeWindowEnd" dataDxfId="2"/>
     <tableColumn id="11" xr3:uid="{F43347B9-3803-4581-9D60-15EA1CBF8049}" name="profile"/>
     <tableColumn id="12" xr3:uid="{1125F421-21B7-48BF-9892-62B15A4C75A5}" name="speedFactor"/>
     <tableColumn id="13" xr3:uid="{EF8C959B-AD29-49C3-8BC7-C2248CA5EC46}" name="fixedCostsTO"/>
@@ -721,7 +728,7 @@
     <tableColumn id="12" xr3:uid="{BCAA728C-CA37-4C53-B92D-9EF80309E6F2}" name="vehicleTypeId"/>
     <tableColumn id="13" xr3:uid="{4D8B07C2-2CD0-47AE-B5F2-DE14A0D1E495}" name="stopDuration"/>
     <tableColumn id="14" xr3:uid="{F659A060-E643-44C3-A792-8818F3219D03}" name="timeWindowProfile"/>
-    <tableColumn id="15" xr3:uid="{9A7BEF9E-1B6C-4967-B0BB-E32D14C703CB}" name="stopDurationAtDepot"/>
+    <tableColumn id="15" xr3:uid="{9A7BEF9E-1B6C-4967-B0BB-E32D14C703CB}" name="stopDurationAtDepo"/>
     <tableColumn id="17" xr3:uid="{B48DC1DF-0D50-4F85-AAF3-709580CFF340}" name="external_costs"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -734,8 +741,8 @@
   <tableColumns count="4">
     <tableColumn id="1" xr3:uid="{C46AC66F-E99B-4596-BCC5-4402F3E497A7}" name="id"/>
     <tableColumn id="4" xr3:uid="{6B9842D9-BAE2-443C-ABB0-F1EA88103531}" name="timeWindowProfileId"/>
-    <tableColumn id="2" xr3:uid="{53D9870D-FCE3-4A00-A402-D21C5687C4F9}" name="timeWindowProfileStart" dataDxfId="5"/>
-    <tableColumn id="3" xr3:uid="{5BA78898-0159-49D6-AD65-F0036067478E}" name="timeWindowProfileEnd" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{53D9870D-FCE3-4A00-A402-D21C5687C4F9}" name="timeWindowProfileStart" dataDxfId="1"/>
+    <tableColumn id="3" xr3:uid="{5BA78898-0159-49D6-AD65-F0036067478E}" name="timeWindowProfileEnd" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1041,7 +1048,7 @@
   <wetp:taskpane dockstate="right" visibility="0" width="438" row="5">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
-  <wetp:taskpane dockstate="right" visibility="0" width="438" row="7">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="6">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1059,19 +1066,24 @@
     <we:property name="14_1jobs" value="&quot;e4ebf57b-1d60ebfd-c740eb9d&quot;"/>
     <we:property name="14_1timeWindowProfiles" value="&quot;f78470fc-c107cc5b-54cc99c0&quot;"/>
     <we:property name="14_1vehicles" value="&quot;8bf81588-6d943fe2-b4f69674&quot;"/>
-    <we:property name="2_1breaks" value="&quot;6b769a54-c276e826-b41f5dbf&quot;"/>
-    <we:property name="2_1depots" value="&quot;40c7738c-7d0d869f-c5c48545&quot;"/>
+    <we:property name="2_1breaks" value="&quot;38d4ff29-04ccf979-2f78ec1e&quot;"/>
+    <we:property name="2_1depots" value="&quot;1359ed08-c54fe70d-9f6f47f6&quot;"/>
     <we:property name="2_1droppedCustomers" value="&quot;352093c7-c9d2b947-ef8e67d7&quot;"/>
-    <we:property name="2_1jobs" value="&quot;50a46a1f-a10ab40c-f5fab965&quot;"/>
+    <we:property name="2_1jobs" value="&quot;120d5110-d064bd46-8b71eb71&quot;"/>
     <we:property name="2_1parameters" value="&quot;fa6a6550-74c811c1-e51c5e81&quot;"/>
     <we:property name="2_1routeDetails" value="&quot;39d70381-db5bf02d-2485588d&quot;"/>
     <we:property name="2_1routeOverview" value="&quot;abd9d53b-efd000b3-a41ffa1f&quot;"/>
-    <we:property name="2_1timeWindowProfiles" value="&quot;05f08bb9-0259b0db-bc32b2ad&quot;"/>
-    <we:property name="2_1vehicles" value="&quot;910a446e-de7f48e3-4d67c1ef&quot;"/>
+    <we:property name="2_1timeWindowProfiles" value="&quot;e5e90b3f-1d0e55cd-c7c07ded&quot;"/>
+    <we:property name="2_1vehicles" value="&quot;669b6949-92ff1d65-08a3ca18&quot;"/>
     <we:property name="2_3breaks" value="&quot;4db2b91d-d67b452b-d5c01d25&quot;"/>
     <we:property name="2_3jobs" value="&quot;1a874645-7b386e0a-81502215&quot;"/>
     <we:property name="2_3timeWindowProfiles" value="&quot;18d160ab-d6668c86-81f62770&quot;"/>
     <we:property name="2_3vehicles" value="&quot;21ef14b5-164df8cc-9e688600&quot;"/>
+    <we:property name="2_1geocodingData" value="&quot;c77a3cbb-e9e5582b-16f64e9b&quot;"/>
+    <we:property name="2_9costAdjustment" value="&quot;f6aae682-fcfa088c-ce2aed51&quot;"/>
+    <we:property name="2_9consolidation" value="&quot;474459be-a211ef10-29185694&quot;"/>
+    <we:property name="2_9shipments" value="&quot;e4762a88-b047b351-e1ecd167&quot;"/>
+    <we:property name="2_9surcharges" value="&quot;46f005e8-be263adb-9777593d&quot;"/>
   </we:properties>
   <we:bindings>
     <we:binding id="3405e038-2cc2c29d-10eabe2d" type="table" appref="{EEC9A2D5-5C2E-4DCE-B266-7F94D3DD210B}"/>
@@ -1083,15 +1095,20 @@
     <we:binding id="1a874645-7b386e0a-81502215" type="table" appref="{F625127A-070D-457C-AED3-12FF1BFBF57C}"/>
     <we:binding id="18d160ab-d6668c86-81f62770" type="table" appref="{F1323060-DFBC-49EA-A93E-8C7031B20F51}"/>
     <we:binding id="4db2b91d-d67b452b-d5c01d25" type="table" appref="{486C6350-B77A-4C63-96A5-7454A2135AC4}"/>
-    <we:binding id="40c7738c-7d0d869f-c5c48545" type="table" appref="{E2CFFF72-7EEF-4987-B318-E23AF7DD55C2}"/>
-    <we:binding id="910a446e-de7f48e3-4d67c1ef" type="table" appref="{CE979D72-3D48-4B73-A4C9-C69944530757}"/>
-    <we:binding id="50a46a1f-a10ab40c-f5fab965" type="table" appref="{89B71074-7E43-4CA4-8F1E-BD90C3E68383}"/>
-    <we:binding id="05f08bb9-0259b0db-bc32b2ad" type="table" appref="{12CD85D8-5F5F-4957-A8E3-475113E9DD6E}"/>
-    <we:binding id="6b769a54-c276e826-b41f5dbf" type="table" appref="{74386F98-86FA-4DBF-AAC5-E42BEE200E06}"/>
     <we:binding id="abd9d53b-efd000b3-a41ffa1f" type="table" appref="{8628E7A6-0BD3-440F-8A2A-11C4FE56BC46}"/>
     <we:binding id="39d70381-db5bf02d-2485588d" type="table" appref="{3EB9D26B-B6C7-49DA-9CCE-3BA567A59802}"/>
     <we:binding id="352093c7-c9d2b947-ef8e67d7" type="table" appref="{BFEB79C1-DF4E-4037-A754-625E127A9F7C}"/>
     <we:binding id="fa6a6550-74c811c1-e51c5e81" type="table" appref="{A0348EC9-5B47-4B03-834D-97D560693932}"/>
+    <we:binding id="1359ed08-c54fe70d-9f6f47f6" type="table" appref="{05D04399-B24C-47D5-ACD7-D551A27BFFCD}"/>
+    <we:binding id="669b6949-92ff1d65-08a3ca18" type="table" appref="{50F11EB6-D2A8-4073-90A3-78287325DEF7}"/>
+    <we:binding id="120d5110-d064bd46-8b71eb71" type="table" appref="{2B2F526E-1566-4E01-A2BD-4A9EF735EFCA}"/>
+    <we:binding id="e5e90b3f-1d0e55cd-c7c07ded" type="table" appref="{0EFB0F73-F884-4932-95E3-6ECA28ADDDEF}"/>
+    <we:binding id="38d4ff29-04ccf979-2f78ec1e" type="table" appref="{C5BD73FB-044C-42D8-B282-788C5760D4B2}"/>
+    <we:binding id="c77a3cbb-e9e5582b-16f64e9b" type="table" appref="{6305A596-FC60-4F34-809C-BA69E5042782}"/>
+    <we:binding id="f6aae682-fcfa088c-ce2aed51" type="table" appref="{72902E3F-BF64-4E6E-AD1A-ECA213809C2B}"/>
+    <we:binding id="474459be-a211ef10-29185694" type="table" appref="{29F3E218-2914-4A4D-9AFA-412719DDE418}"/>
+    <we:binding id="e4762a88-b047b351-e1ecd167" type="table" appref="{1CE20A09-E773-4782-A78A-4AA0146718AC}"/>
+    <we:binding id="46f005e8-be263adb-9777593d" type="table" appref="{A0799751-F80F-4C37-B636-EDA70F5D9276}"/>
   </we:bindings>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </we:webextension>
@@ -1102,26 +1119,26 @@
   <we:reference id="e504fb41-a92a-4526-b101-542f357b7983" version="1.0.0.0" store="\\LAPTOP-ULOOTDBM\Manifest" storeType="Filesystem"/>
   <we:alternateReferences/>
   <we:properties>
-    <we:property name="2_1breaks" value="&quot;bade92af-f7d4abb8-dfbd0975&quot;"/>
-    <we:property name="2_1depots" value="&quot;2c2d3475-cc0c5c3d-f3adb6ec&quot;"/>
+    <we:property name="2_1breaks" value="&quot;50037b50-9ef149ed-d1064bde&quot;"/>
+    <we:property name="2_1depots" value="&quot;2bb0595a-4f58da39-7857f3f8&quot;"/>
     <we:property name="2_1droppedCustomers" value="&quot;fc401730-040504bf-d448b086&quot;"/>
-    <we:property name="2_1jobs" value="&quot;22f3687a-a1c2606c-83b46295&quot;"/>
+    <we:property name="2_1jobs" value="&quot;ce8d0eff-92dec9a9-132de410&quot;"/>
     <we:property name="2_1parameters" value="&quot;44c77af5-a430caf3-1dbe6577&quot;"/>
     <we:property name="2_1routeDetails" value="&quot;37a755cb-87a0ed7f-a220640d&quot;"/>
     <we:property name="2_1routeOverview" value="&quot;53b148c5-6be943f6-0b4ca14a&quot;"/>
-    <we:property name="2_1timeWindowProfiles" value="&quot;c2c73dad-e948b378-52853065&quot;"/>
-    <we:property name="2_1vehicles" value="&quot;0ec1d9a8-ce8e9fc6-49dfdcdd&quot;"/>
+    <we:property name="2_1timeWindowProfiles" value="&quot;33b44c92-cd38843d-686e23bd&quot;"/>
+    <we:property name="2_1vehicles" value="&quot;ff9850ad-4ccb6c11-449d01ff&quot;"/>
   </we:properties>
   <we:bindings>
-    <we:binding id="2c2d3475-cc0c5c3d-f3adb6ec" type="matrix" appref="{63A1049B-A37B-42B2-83D0-D48F45C21354}"/>
-    <we:binding id="0ec1d9a8-ce8e9fc6-49dfdcdd" type="matrix" appref="{C55476B0-0DB4-446B-AF8D-421E2CD128D7}"/>
-    <we:binding id="22f3687a-a1c2606c-83b46295" type="matrix" appref="{B09183C9-7DA5-430B-9EC5-F08C28B2D708}"/>
-    <we:binding id="c2c73dad-e948b378-52853065" type="matrix" appref="{6322DE5F-8152-4E29-90D0-8A92B177DC60}"/>
-    <we:binding id="bade92af-f7d4abb8-dfbd0975" type="matrix" appref="{5710F216-2749-4C81-A85C-137BDBFBBD2C}"/>
     <we:binding id="53b148c5-6be943f6-0b4ca14a" type="table" appref="{43A7F7FF-B89E-4C54-97C2-58D1AD93BC65}"/>
     <we:binding id="fc401730-040504bf-d448b086" type="table" appref="{70DE82A1-4A35-4D9F-828A-CB10E820B8C2}"/>
     <we:binding id="37a755cb-87a0ed7f-a220640d" type="table" appref="{F11DBFB7-7701-48D3-91F4-293D6D8705B0}"/>
     <we:binding id="44c77af5-a430caf3-1dbe6577" type="table" appref="{983A8470-2E0A-4B62-B7B1-44C5997C0F9E}"/>
+    <we:binding id="2bb0595a-4f58da39-7857f3f8" type="table" appref="{FFF172BB-1408-43EA-BC08-DA3FCBD98F4E}"/>
+    <we:binding id="ff9850ad-4ccb6c11-449d01ff" type="table" appref="{F578D03B-963E-4508-BD5E-D7704F4601A4}"/>
+    <we:binding id="ce8d0eff-92dec9a9-132de410" type="table" appref="{0A9385AC-1D15-4819-AF7F-B5F2B51852E2}"/>
+    <we:binding id="33b44c92-cd38843d-686e23bd" type="table" appref="{BEFAB9D5-C695-4FBA-9551-2644803626BA}"/>
+    <we:binding id="50037b50-9ef149ed-d1064bde" type="table" appref="{9221A3C4-73AB-4958-8C7B-FD661E075CA0}"/>
   </we:bindings>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </we:webextension>
@@ -1132,7 +1149,7 @@
   <dimension ref="A1:G5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
+      <selection activeCell="B2" sqref="B2:G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1152,19 +1169,19 @@
         <v>131</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>143</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>144</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="F1" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="G1" s="2" t="s">
         <v>145</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>149</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>146</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.3">
@@ -1218,7 +1235,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>2</v>
@@ -1241,7 +1258,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>2</v>
@@ -1295,21 +1312,6 @@
         <x15:webExtension appRef="{486C6350-B77A-4C63-96A5-7454A2135AC4}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
-        <x15:webExtension appRef="{63A1049B-A37B-42B2-83D0-D48F45C21354}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{C55476B0-0DB4-446B-AF8D-421E2CD128D7}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{B09183C9-7DA5-430B-9EC5-F08C28B2D708}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{6322DE5F-8152-4E29-90D0-8A92B177DC60}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{5710F216-2749-4C81-A85C-137BDBFBBD2C}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
         <x15:webExtension appRef="{43A7F7FF-B89E-4C54-97C2-58D1AD93BC65}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
@@ -1320,21 +1322,6 @@
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
         <x15:webExtension appRef="{983A8470-2E0A-4B62-B7B1-44C5997C0F9E}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{E2CFFF72-7EEF-4987-B318-E23AF7DD55C2}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{CE979D72-3D48-4B73-A4C9-C69944530757}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{89B71074-7E43-4CA4-8F1E-BD90C3E68383}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{12CD85D8-5F5F-4957-A8E3-475113E9DD6E}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{74386F98-86FA-4DBF-AAC5-E42BEE200E06}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
         <x15:webExtension appRef="{8628E7A6-0BD3-440F-8A2A-11C4FE56BC46}">
@@ -1349,6 +1336,33 @@
         <x15:webExtension appRef="{A0348EC9-5B47-4B03-834D-97D560693932}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
+        <x15:webExtension appRef="{05D04399-B24C-47D5-ACD7-D551A27BFFCD}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{50F11EB6-D2A8-4073-90A3-78287325DEF7}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{2B2F526E-1566-4E01-A2BD-4A9EF735EFCA}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{0EFB0F73-F884-4932-95E3-6ECA28ADDDEF}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{C5BD73FB-044C-42D8-B282-788C5760D4B2}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{72902E3F-BF64-4E6E-AD1A-ECA213809C2B}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{29F3E218-2914-4A4D-9AFA-412719DDE418}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{1CE20A09-E773-4782-A78A-4AA0146718AC}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{A0799751-F80F-4C37-B636-EDA70F5D9276}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
       </x15:webExtensions>
     </ext>
   </extLst>
@@ -1360,7 +1374,7 @@
   <dimension ref="A1:H2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H10" sqref="H10"/>
+      <selection activeCell="J11" sqref="J11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1391,7 +1405,7 @@
         <v>116</v>
       </c>
       <c r="H1" s="2" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.3">
@@ -1432,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731114BF-9A8C-4E2B-8661-4204E3E4B0F3}">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+    <sheetView topLeftCell="P1" workbookViewId="0">
+      <selection activeCell="B2" sqref="B2:V16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1451,11 +1465,14 @@
     <col min="11" max="11" width="18.33203125" bestFit="1" customWidth="1"/>
     <col min="12" max="12" width="8.6640625" bestFit="1" customWidth="1"/>
     <col min="13" max="13" width="13.88671875" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="7.5546875" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17.33203125" customWidth="1"/>
     <col min="15" max="15" width="10.5546875" bestFit="1" customWidth="1"/>
     <col min="16" max="16" width="16.88671875" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="10.21875" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="13.6640625" customWidth="1"/>
+    <col min="17" max="17" width="14.88671875" customWidth="1"/>
+    <col min="18" max="18" width="25.88671875" customWidth="1"/>
+    <col min="19" max="19" width="22.21875" customWidth="1"/>
+    <col min="20" max="20" width="16.44140625" customWidth="1"/>
+    <col min="21" max="21" width="32.77734375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:22" ht="15" thickTop="1" x14ac:dyDescent="0.3">
@@ -1499,28 +1516,28 @@
         <v>128</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>129</v>
       </c>
       <c r="P1" s="2" t="s">
+        <v>152</v>
+      </c>
+      <c r="Q1" s="2" t="s">
+        <v>156</v>
+      </c>
+      <c r="R1" s="2" t="s">
         <v>153</v>
-      </c>
-      <c r="Q1" s="2" t="s">
-        <v>157</v>
-      </c>
-      <c r="R1" s="2" t="s">
-        <v>154</v>
       </c>
       <c r="S1" s="2" t="s">
         <v>130</v>
       </c>
       <c r="T1" s="2" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="U1" s="2" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="V1" s="2" t="s">
         <v>131</v>
@@ -1795,7 +1812,7 @@
         <v>100</v>
       </c>
       <c r="V5" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="6" spans="1:22" x14ac:dyDescent="0.3">
@@ -1863,7 +1880,7 @@
         <v>100</v>
       </c>
       <c r="V6" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="7" spans="1:22" x14ac:dyDescent="0.3">
@@ -1931,7 +1948,7 @@
         <v>100</v>
       </c>
       <c r="V7" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
     </row>
     <row r="8" spans="1:22" x14ac:dyDescent="0.3">
@@ -2562,8 +2579,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{17E9840B-7203-4504-8A3D-5B22E03396E5}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:Q45"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="P1" sqref="P1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2625,11 +2642,11 @@
       <c r="O1" s="2" t="s">
         <v>139</v>
       </c>
-      <c r="P1" s="6" t="s">
-        <v>140</v>
+      <c r="P1" s="7" t="s">
+        <v>157</v>
       </c>
       <c r="Q1" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
     </row>
     <row r="2" spans="1:17" x14ac:dyDescent="0.3">
@@ -4993,13 +5010,13 @@
         <v>111</v>
       </c>
       <c r="B1" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>141</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>142</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>143</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.3">
@@ -5147,15 +5164,40 @@
   <tableParts count="1">
     <tablePart r:id="rId1"/>
   </tableParts>
+  <extLst>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{F7C9EE02-42E1-4005-9D12-6889AFFD525C}">
+      <x15:webExtensions xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
+        <x15:webExtension appRef="{FFF172BB-1408-43EA-BC08-DA3FCBD98F4E}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{F578D03B-963E-4508-BD5E-D7704F4601A4}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{0A9385AC-1D15-4819-AF7F-B5F2B51852E2}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{BEFAB9D5-C695-4FBA-9551-2644803626BA}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{9221A3C4-73AB-4958-8C7B-FD661E075CA0}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{6305A596-FC60-4F34-809C-BA69E5042782}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+      </x15:webExtensions>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1bb9a224-31c7-42e8-a065-e7e76b1c03c9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5380,27 +5422,17 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1bb9a224-31c7-42e8-a065-e7e76b1c03c9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B9BDB6-33A2-4400-8419-C415F30CCE55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1031B672-90B3-497E-AD74-4A5D391605E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1bb9a224-31c7-42e8-a065-e7e76b1c03c9"/>
-    <ds:schemaRef ds:uri="15a9d969-c72e-439c-8c09-437e8295500b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5425,9 +5457,18 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1031B672-90B3-497E-AD74-4A5D391605E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B9BDB6-33A2-4400-8419-C415F30CCE55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1bb9a224-31c7-42e8-a065-e7e76b1c03c9"/>
+    <ds:schemaRef ds:uri="15a9d969-c72e-439c-8c09-437e8295500b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
changed a column name in Milkrun
</commit_message>
<xml_diff>
--- a/pyloghub/sample_data/MilkrunPlusSampleDataAddresses.xlsx
+++ b/pyloghub/sample_data/MilkrunPlusSampleDataAddresses.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\git\log-hub-python\pyloghub\sample_data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09AAAB2A-C4F1-44BF-88AA-38EEA1D4E70D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EFD6FDC-A443-4E4E-9027-65FA10F69FB9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="4" activeTab="4" xr2:uid="{0F815C8C-0ED9-4734-BB11-57244BED7296}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" firstSheet="1" activeTab="2" xr2:uid="{0F815C8C-0ED9-4734-BB11-57244BED7296}"/>
   </bookViews>
   <sheets>
     <sheet name="breaks" sheetId="7" r:id="rId1"/>
@@ -507,13 +507,13 @@
     <t>maximumDistanceBetweenStops</t>
   </si>
   <si>
-    <t>fixedCostsTO</t>
-  </si>
-  <si>
     <t>costPerStop</t>
   </si>
   <si>
     <t>stopDurationAtDepo</t>
+  </si>
+  <si>
+    <t>fixed</t>
   </si>
 </sst>
 </file>
@@ -695,7 +695,7 @@
     <tableColumn id="10" xr3:uid="{AA4E50FA-44AD-4DEE-ABFC-F84CDE509891}" name="timeWindowEnd" dataDxfId="2"/>
     <tableColumn id="11" xr3:uid="{F43347B9-3803-4581-9D60-15EA1CBF8049}" name="profile"/>
     <tableColumn id="12" xr3:uid="{1125F421-21B7-48BF-9892-62B15A4C75A5}" name="speedFactor"/>
-    <tableColumn id="13" xr3:uid="{EF8C959B-AD29-49C3-8BC7-C2248CA5EC46}" name="fixedCostsTO"/>
+    <tableColumn id="13" xr3:uid="{EF8C959B-AD29-49C3-8BC7-C2248CA5EC46}" name="fixed"/>
     <tableColumn id="14" xr3:uid="{0320C09B-8370-490B-AE50-E6246943B7C3}" name="perHour"/>
     <tableColumn id="19" xr3:uid="{62F377B8-BDFE-4C88-A6EF-E480A17D35E1}" name="perKilometer"/>
     <tableColumn id="18" xr3:uid="{6E69B321-9621-4D6E-B178-6DCCBB90DFCB}" name="costPerStop"/>
@@ -1048,7 +1048,7 @@
   <wetp:taskpane dockstate="right" visibility="0" width="438" row="5">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
   </wetp:taskpane>
-  <wetp:taskpane dockstate="right" visibility="0" width="438" row="6">
+  <wetp:taskpane dockstate="right" visibility="0" width="438" row="5">
     <wetp:webextensionref xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
   </wetp:taskpane>
 </wetp:taskpanes>
@@ -1119,26 +1119,26 @@
   <we:reference id="e504fb41-a92a-4526-b101-542f357b7983" version="1.0.0.0" store="\\LAPTOP-ULOOTDBM\Manifest" storeType="Filesystem"/>
   <we:alternateReferences/>
   <we:properties>
-    <we:property name="2_1breaks" value="&quot;50037b50-9ef149ed-d1064bde&quot;"/>
-    <we:property name="2_1depots" value="&quot;2bb0595a-4f58da39-7857f3f8&quot;"/>
-    <we:property name="2_1droppedCustomers" value="&quot;fc401730-040504bf-d448b086&quot;"/>
-    <we:property name="2_1jobs" value="&quot;ce8d0eff-92dec9a9-132de410&quot;"/>
-    <we:property name="2_1parameters" value="&quot;44c77af5-a430caf3-1dbe6577&quot;"/>
-    <we:property name="2_1routeDetails" value="&quot;37a755cb-87a0ed7f-a220640d&quot;"/>
-    <we:property name="2_1routeOverview" value="&quot;53b148c5-6be943f6-0b4ca14a&quot;"/>
-    <we:property name="2_1timeWindowProfiles" value="&quot;33b44c92-cd38843d-686e23bd&quot;"/>
-    <we:property name="2_1vehicles" value="&quot;ff9850ad-4ccb6c11-449d01ff&quot;"/>
+    <we:property name="2_1breaks" value="&quot;b20ac0d2-e9504b51-0deaf588&quot;"/>
+    <we:property name="2_1depots" value="&quot;d3c00983-b69dfeb3-e2303157&quot;"/>
+    <we:property name="2_1droppedCustomers" value="&quot;0dbeba3d-c5fede97-47ba6c0f&quot;"/>
+    <we:property name="2_1jobs" value="&quot;d0c012d4-a244f84d-e5c9cccc&quot;"/>
+    <we:property name="2_1parameters" value="&quot;f20f542e-34ba5409-71e089f4&quot;"/>
+    <we:property name="2_1routeDetails" value="&quot;ee6f1cef-943abb87-d33c6609&quot;"/>
+    <we:property name="2_1routeOverview" value="&quot;1a217bb9-1031b964-563f4218&quot;"/>
+    <we:property name="2_1timeWindowProfiles" value="&quot;2f50a317-91b3c6ab-10563de9&quot;"/>
+    <we:property name="2_1vehicles" value="&quot;f0e6ef63-acd29834-2999e0c5&quot;"/>
   </we:properties>
   <we:bindings>
-    <we:binding id="53b148c5-6be943f6-0b4ca14a" type="table" appref="{43A7F7FF-B89E-4C54-97C2-58D1AD93BC65}"/>
-    <we:binding id="fc401730-040504bf-d448b086" type="table" appref="{70DE82A1-4A35-4D9F-828A-CB10E820B8C2}"/>
-    <we:binding id="37a755cb-87a0ed7f-a220640d" type="table" appref="{F11DBFB7-7701-48D3-91F4-293D6D8705B0}"/>
-    <we:binding id="44c77af5-a430caf3-1dbe6577" type="table" appref="{983A8470-2E0A-4B62-B7B1-44C5997C0F9E}"/>
-    <we:binding id="2bb0595a-4f58da39-7857f3f8" type="table" appref="{FFF172BB-1408-43EA-BC08-DA3FCBD98F4E}"/>
-    <we:binding id="ff9850ad-4ccb6c11-449d01ff" type="table" appref="{F578D03B-963E-4508-BD5E-D7704F4601A4}"/>
-    <we:binding id="ce8d0eff-92dec9a9-132de410" type="table" appref="{0A9385AC-1D15-4819-AF7F-B5F2B51852E2}"/>
-    <we:binding id="33b44c92-cd38843d-686e23bd" type="table" appref="{BEFAB9D5-C695-4FBA-9551-2644803626BA}"/>
-    <we:binding id="50037b50-9ef149ed-d1064bde" type="table" appref="{9221A3C4-73AB-4958-8C7B-FD661E075CA0}"/>
+    <we:binding id="d3c00983-b69dfeb3-e2303157" type="table" appref="{C0B6EF2B-DDF5-4899-82EA-0B3C1D3EEFC9}"/>
+    <we:binding id="f0e6ef63-acd29834-2999e0c5" type="table" appref="{9421BCE5-D04C-42FE-BD5F-B1EA023DD5F2}"/>
+    <we:binding id="d0c012d4-a244f84d-e5c9cccc" type="table" appref="{3D3C343C-399E-4E45-9E93-AB558841BDF2}"/>
+    <we:binding id="2f50a317-91b3c6ab-10563de9" type="table" appref="{1B161061-844E-4609-92A0-C1E7FADD0FF7}"/>
+    <we:binding id="b20ac0d2-e9504b51-0deaf588" type="table" appref="{5937B5AC-6C76-4A8E-9CC0-A38788912DBD}"/>
+    <we:binding id="1a217bb9-1031b964-563f4218" type="table" appref="{11BBF86E-2586-41EA-908B-850AF7C73D6D}"/>
+    <we:binding id="ee6f1cef-943abb87-d33c6609" type="table" appref="{59DAB5B0-70CD-4ABA-9B4A-F44CE8227D23}"/>
+    <we:binding id="0dbeba3d-c5fede97-47ba6c0f" type="table" appref="{0563FF3F-19FC-4AB0-86CB-7B903B5169D6}"/>
+    <we:binding id="f20f542e-34ba5409-71e089f4" type="table" appref="{0E10238D-641A-435F-A5E5-C87A36FC748E}"/>
   </we:bindings>
   <we:snapshot xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships"/>
 </we:webextension>
@@ -1310,18 +1310,6 @@
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
         <x15:webExtension appRef="{486C6350-B77A-4C63-96A5-7454A2135AC4}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{43A7F7FF-B89E-4C54-97C2-58D1AD93BC65}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{70DE82A1-4A35-4D9F-828A-CB10E820B8C2}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{F11DBFB7-7701-48D3-91F4-293D6D8705B0}">
-          <xm:f>#REF!</xm:f>
-        </x15:webExtension>
-        <x15:webExtension appRef="{983A8470-2E0A-4B62-B7B1-44C5997C0F9E}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
         <x15:webExtension appRef="{8628E7A6-0BD3-440F-8A2A-11C4FE56BC46}">
@@ -1363,6 +1351,18 @@
         <x15:webExtension appRef="{A0799751-F80F-4C37-B636-EDA70F5D9276}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
+        <x15:webExtension appRef="{11BBF86E-2586-41EA-908B-850AF7C73D6D}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{59DAB5B0-70CD-4ABA-9B4A-F44CE8227D23}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{0563FF3F-19FC-4AB0-86CB-7B903B5169D6}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
+        <x15:webExtension appRef="{0E10238D-641A-435F-A5E5-C87A36FC748E}">
+          <xm:f>#REF!</xm:f>
+        </x15:webExtension>
       </x15:webExtensions>
     </ext>
   </extLst>
@@ -1446,8 +1446,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{731114BF-9A8C-4E2B-8661-4204E3E4B0F3}">
   <dimension ref="A1:V23"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:V16"/>
+    <sheetView tabSelected="1" topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1516,7 +1516,7 @@
         <v>128</v>
       </c>
       <c r="N1" s="2" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="O1" s="2" t="s">
         <v>129</v>
@@ -1525,7 +1525,7 @@
         <v>152</v>
       </c>
       <c r="Q1" s="2" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="R1" s="2" t="s">
         <v>153</v>
@@ -2643,7 +2643,7 @@
         <v>139</v>
       </c>
       <c r="P1" s="7" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="Q1" t="s">
         <v>151</v>
@@ -4993,7 +4993,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{41DC451B-53B4-41CD-9364-638505779A88}">
   <dimension ref="A1:D11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="B2" sqref="B2:D11"/>
     </sheetView>
   </sheetViews>
@@ -5167,22 +5167,22 @@
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{F7C9EE02-42E1-4005-9D12-6889AFFD525C}">
       <x15:webExtensions xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main">
-        <x15:webExtension appRef="{FFF172BB-1408-43EA-BC08-DA3FCBD98F4E}">
+        <x15:webExtension appRef="{6305A596-FC60-4F34-809C-BA69E5042782}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
-        <x15:webExtension appRef="{F578D03B-963E-4508-BD5E-D7704F4601A4}">
+        <x15:webExtension appRef="{C0B6EF2B-DDF5-4899-82EA-0B3C1D3EEFC9}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
-        <x15:webExtension appRef="{0A9385AC-1D15-4819-AF7F-B5F2B51852E2}">
+        <x15:webExtension appRef="{9421BCE5-D04C-42FE-BD5F-B1EA023DD5F2}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
-        <x15:webExtension appRef="{BEFAB9D5-C695-4FBA-9551-2644803626BA}">
+        <x15:webExtension appRef="{3D3C343C-399E-4E45-9E93-AB558841BDF2}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
-        <x15:webExtension appRef="{9221A3C4-73AB-4958-8C7B-FD661E075CA0}">
+        <x15:webExtension appRef="{1B161061-844E-4609-92A0-C1E7FADD0FF7}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
-        <x15:webExtension appRef="{6305A596-FC60-4F34-809C-BA69E5042782}">
+        <x15:webExtension appRef="{5937B5AC-6C76-4A8E-9CC0-A38788912DBD}">
           <xm:f>#REF!</xm:f>
         </x15:webExtension>
       </x15:webExtensions>
@@ -5192,12 +5192,11 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1bb9a224-31c7-42e8-a065-e7e76b1c03c9" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -5422,17 +5421,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1bb9a224-31c7-42e8-a065-e7e76b1c03c9" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1031B672-90B3-497E-AD74-4A5D391605E1}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B9BDB6-33A2-4400-8419-C415F30CCE55}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="1bb9a224-31c7-42e8-a065-e7e76b1c03c9"/>
+    <ds:schemaRef ds:uri="15a9d969-c72e-439c-8c09-437e8295500b"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -5457,18 +5466,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{19B9BDB6-33A2-4400-8419-C415F30CCE55}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{1031B672-90B3-497E-AD74-4A5D391605E1}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="1bb9a224-31c7-42e8-a065-e7e76b1c03c9"/>
-    <ds:schemaRef ds:uri="15a9d969-c72e-439c-8c09-437e8295500b"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>